<commit_message>
mapeamento dos campos com dependencia
</commit_message>
<xml_diff>
--- a/importar-parceiro.xlsx
+++ b/importar-parceiro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\Contmatic\erp-web\src\assets\arquivos-download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manuela.silva\Desktop\python-cadastros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA65A8DD-042A-41AB-85CB-58CBAFACB18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986460CD-59E0-4ECA-9E5B-8B1678F594AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="importar-parceiros" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <r>
       <rPr>
@@ -139,398 +139,416 @@
     <t>Inscrição Municipal</t>
   </si>
   <si>
-    <t>Inscrição Estadual</t>
-  </si>
-  <si>
-    <t>SUFRAMA</t>
-  </si>
-  <si>
-    <t>Nome do Contato</t>
-  </si>
-  <si>
-    <t>CPF/CNPJ contato</t>
-  </si>
-  <si>
-    <t>Área responsável</t>
-  </si>
-  <si>
-    <t>Recebe XML</t>
-  </si>
-  <si>
-    <t>Tipo de telefone</t>
-  </si>
-  <si>
-    <t>Telefone de contato</t>
-  </si>
-  <si>
-    <t>E-mail de contato</t>
-  </si>
-  <si>
-    <t>Tipo de Endereço</t>
-  </si>
-  <si>
-    <t>CEP</t>
-  </si>
-  <si>
-    <t>Logradouro</t>
-  </si>
-  <si>
-    <t>Número</t>
-  </si>
-  <si>
-    <t>Complemento</t>
-  </si>
-  <si>
-    <t>Município</t>
-  </si>
-  <si>
-    <t>Bairro</t>
-  </si>
-  <si>
-    <t>UF</t>
-  </si>
-  <si>
-    <t>País</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UFs </t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>DF</t>
-  </si>
-  <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT </t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>PB</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>PI</t>
-  </si>
-  <si>
-    <t>PR</t>
-  </si>
-  <si>
-    <t>RJ</t>
-  </si>
-  <si>
-    <t>RN</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>RR</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-  <si>
-    <t>UNIDADE DE MEDIDA</t>
-  </si>
-  <si>
-    <t>ORIGEM</t>
-  </si>
-  <si>
-    <t>TIPO DO PRODUTO</t>
-  </si>
-  <si>
-    <t>AMPOLA</t>
-  </si>
-  <si>
-    <t>0 - Nacional: exceto as indicadas nos códigos 3, 4, 5 e 8</t>
-  </si>
-  <si>
-    <t>00 - Mercadoria para Revenda</t>
-  </si>
-  <si>
-    <t>BALDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Estrangeira: importação direta, exceto a indicada no código 6 </t>
-  </si>
-  <si>
-    <t>01 - Matéria Prima</t>
-  </si>
-  <si>
-    <t>BANDEJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 - Estrangeira: adquirida no mercado interno, exceto a indicada no código 7  </t>
-  </si>
-  <si>
-    <t>02 - Embalagens</t>
-  </si>
-  <si>
-    <t>BARRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 - Nacional: mercadoria ou bem com Conteúdo de Importação superior a 40% e inferior ou igual a 70% </t>
-  </si>
-  <si>
-    <t>03 - Produto em Processo</t>
-  </si>
-  <si>
-    <t>BISNAG</t>
-  </si>
-  <si>
-    <t>4 - Nacional: produção em conformidade com processos básicos tratados na legislação dos Ajustes</t>
-  </si>
-  <si>
-    <t>04 - Produto Acabado</t>
-  </si>
-  <si>
-    <t>BLOCO</t>
-  </si>
-  <si>
-    <t>5 - Nacional: mercadoria ou bem com Conteúdo de Importação inferior ou igual a 40%</t>
-  </si>
-  <si>
-    <t>05 - Subproduto</t>
-  </si>
-  <si>
-    <t>BOBINA</t>
-  </si>
-  <si>
-    <t>6 - Estrangeira: importação direta, sem similar nacional, constante em lista da CAMEX</t>
-  </si>
-  <si>
-    <t>06 - Produto Intermediário</t>
-  </si>
-  <si>
-    <t>BOMB</t>
-  </si>
-  <si>
-    <t>7 - Estrangeira: adquirida no mercado interno, sem similar nacional, constante em lista da CAMEX</t>
-  </si>
-  <si>
-    <t>07 - Material de uso e consumo</t>
-  </si>
-  <si>
-    <t>CAPS</t>
-  </si>
-  <si>
-    <t>8 - Nacional: mercadoria ou bem com Conteúdo de Importação superior a 70%</t>
-  </si>
-  <si>
-    <t>08 - Ativo Imobilizado</t>
-  </si>
-  <si>
-    <t>CART</t>
-  </si>
-  <si>
-    <t>10 - Outros Insumos</t>
-  </si>
-  <si>
-    <t>CENTO</t>
-  </si>
-  <si>
-    <t>99 - Outros</t>
-  </si>
-  <si>
-    <t>CJ</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>CM2</t>
-  </si>
-  <si>
-    <t>CX</t>
-  </si>
-  <si>
-    <t>CX2</t>
-  </si>
-  <si>
-    <t>CX3</t>
-  </si>
-  <si>
-    <t>CX5</t>
-  </si>
-  <si>
-    <t>CX10</t>
-  </si>
-  <si>
-    <t>CX15</t>
-  </si>
-  <si>
-    <t>CX20</t>
-  </si>
-  <si>
-    <t>CX25</t>
-  </si>
-  <si>
-    <t>CX50</t>
-  </si>
-  <si>
-    <t>CX100</t>
-  </si>
-  <si>
-    <t>DISP</t>
-  </si>
-  <si>
-    <t>DUZIA</t>
-  </si>
-  <si>
-    <t>EMBAL</t>
-  </si>
-  <si>
-    <t>FARDO</t>
-  </si>
-  <si>
-    <t>FOLHA</t>
-  </si>
-  <si>
-    <t>FRASCO</t>
-  </si>
-  <si>
-    <t>GALAO</t>
-  </si>
-  <si>
-    <t>GF</t>
-  </si>
-  <si>
-    <t>GRAMAS</t>
-  </si>
-  <si>
-    <t>JOGO</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>KIT</t>
-  </si>
-  <si>
-    <t>LATA</t>
-  </si>
-  <si>
-    <t>LITRO</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>MILHEI</t>
-  </si>
-  <si>
-    <t>ML</t>
-  </si>
-  <si>
-    <t>MWH</t>
-  </si>
-  <si>
-    <t>PACOTE</t>
-  </si>
-  <si>
-    <t>PALETE</t>
-  </si>
-  <si>
-    <t>PARES</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>POTE</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>RESMA</t>
-  </si>
-  <si>
-    <t>ROLO</t>
-  </si>
-  <si>
-    <t>SACO</t>
-  </si>
-  <si>
-    <t>SACOLA</t>
-  </si>
-  <si>
-    <t>TAMBOR</t>
-  </si>
-  <si>
-    <t>TANQUE</t>
-  </si>
-  <si>
-    <t>TON</t>
-  </si>
-  <si>
-    <t>TUBO</t>
-  </si>
-  <si>
-    <t>UNID</t>
-  </si>
-  <si>
-    <t>VASIL</t>
-  </si>
-  <si>
-    <t>VIDRO</t>
-  </si>
-  <si>
     <t>Tipo de Inscrição Estadual
 (obrigatório)</t>
+  </si>
+  <si>
+    <t>Inscrição Estadual</t>
+  </si>
+  <si>
+    <t>SUFRAMA</t>
+  </si>
+  <si>
+    <t>Nome do Contato</t>
+  </si>
+  <si>
+    <t>CPF/CNPJ contato</t>
+  </si>
+  <si>
+    <t>Área responsável</t>
+  </si>
+  <si>
+    <t>Recebe XML</t>
+  </si>
+  <si>
+    <t>Tipo de telefone</t>
+  </si>
+  <si>
+    <t>Telefone de contato</t>
+  </si>
+  <si>
+    <t>E-mail de contato</t>
+  </si>
+  <si>
+    <t>Tipo de Endereço</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>Logradouro</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>Município</t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Ativo</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFs </t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT </t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>UNIDADE DE MEDIDA</t>
+  </si>
+  <si>
+    <t>ORIGEM</t>
+  </si>
+  <si>
+    <t>TIPO DO PRODUTO</t>
+  </si>
+  <si>
+    <t>AMPOLA</t>
+  </si>
+  <si>
+    <t>0 - Nacional: exceto as indicadas nos códigos 3, 4, 5 e 8</t>
+  </si>
+  <si>
+    <t>00 - Mercadoria para Revenda</t>
+  </si>
+  <si>
+    <t>BALDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Estrangeira: importação direta, exceto a indicada no código 6 </t>
+  </si>
+  <si>
+    <t>01 - Matéria Prima</t>
+  </si>
+  <si>
+    <t>BANDEJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - Estrangeira: adquirida no mercado interno, exceto a indicada no código 7  </t>
+  </si>
+  <si>
+    <t>02 - Embalagens</t>
+  </si>
+  <si>
+    <t>BARRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 - Nacional: mercadoria ou bem com Conteúdo de Importação superior a 40% e inferior ou igual a 70% </t>
+  </si>
+  <si>
+    <t>03 - Produto em Processo</t>
+  </si>
+  <si>
+    <t>BISNAG</t>
+  </si>
+  <si>
+    <t>4 - Nacional: produção em conformidade com processos básicos tratados na legislação dos Ajustes</t>
+  </si>
+  <si>
+    <t>04 - Produto Acabado</t>
+  </si>
+  <si>
+    <t>BLOCO</t>
+  </si>
+  <si>
+    <t>5 - Nacional: mercadoria ou bem com Conteúdo de Importação inferior ou igual a 40%</t>
+  </si>
+  <si>
+    <t>05 - Subproduto</t>
+  </si>
+  <si>
+    <t>BOBINA</t>
+  </si>
+  <si>
+    <t>6 - Estrangeira: importação direta, sem similar nacional, constante em lista da CAMEX</t>
+  </si>
+  <si>
+    <t>06 - Produto Intermediário</t>
+  </si>
+  <si>
+    <t>BOMB</t>
+  </si>
+  <si>
+    <t>7 - Estrangeira: adquirida no mercado interno, sem similar nacional, constante em lista da CAMEX</t>
+  </si>
+  <si>
+    <t>07 - Material de uso e consumo</t>
+  </si>
+  <si>
+    <t>CAPS</t>
+  </si>
+  <si>
+    <t>8 - Nacional: mercadoria ou bem com Conteúdo de Importação superior a 70%</t>
+  </si>
+  <si>
+    <t>08 - Ativo Imobilizado</t>
+  </si>
+  <si>
+    <t>CART</t>
+  </si>
+  <si>
+    <t>10 - Outros Insumos</t>
+  </si>
+  <si>
+    <t>CENTO</t>
+  </si>
+  <si>
+    <t>99 - Outros</t>
+  </si>
+  <si>
+    <t>CJ</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CM2</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>CX2</t>
+  </si>
+  <si>
+    <t>CX3</t>
+  </si>
+  <si>
+    <t>CX5</t>
+  </si>
+  <si>
+    <t>CX10</t>
+  </si>
+  <si>
+    <t>CX15</t>
+  </si>
+  <si>
+    <t>CX20</t>
+  </si>
+  <si>
+    <t>CX25</t>
+  </si>
+  <si>
+    <t>CX50</t>
+  </si>
+  <si>
+    <t>CX100</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>DUZIA</t>
+  </si>
+  <si>
+    <t>EMBAL</t>
+  </si>
+  <si>
+    <t>FARDO</t>
+  </si>
+  <si>
+    <t>FOLHA</t>
+  </si>
+  <si>
+    <t>FRASCO</t>
+  </si>
+  <si>
+    <t>GALAO</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>GRAMAS</t>
+  </si>
+  <si>
+    <t>JOGO</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>KIT</t>
+  </si>
+  <si>
+    <t>LATA</t>
+  </si>
+  <si>
+    <t>LITRO</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>MILHEI</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MWH</t>
+  </si>
+  <si>
+    <t>PACOTE</t>
+  </si>
+  <si>
+    <t>PALETE</t>
+  </si>
+  <si>
+    <t>PARES</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>POTE</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>RESMA</t>
+  </si>
+  <si>
+    <t>ROLO</t>
+  </si>
+  <si>
+    <t>SACO</t>
+  </si>
+  <si>
+    <t>SACOLA</t>
+  </si>
+  <si>
+    <t>TAMBOR</t>
+  </si>
+  <si>
+    <t>TANQUE</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>TUBO</t>
+  </si>
+  <si>
+    <t>UNID</t>
+  </si>
+  <si>
+    <t>VASIL</t>
+  </si>
+  <si>
+    <t>VIDRO</t>
+  </si>
+  <si>
+    <t>Pessoa Jurídica</t>
+  </si>
+  <si>
+    <t>Isento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	92.754.738/0001-62</t>
+  </si>
+  <si>
+    <t>Renner Teste</t>
   </si>
 </sst>
 </file>
@@ -773,10 +791,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1156,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1166,34 +1184,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="50.140625" style="2" customWidth="1"/>
     <col min="3" max="4" width="50.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="41.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="52.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="52.5703125" style="4" customWidth="1"/>
-    <col min="9" max="13" width="52.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="52.5703125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="52.5703125" style="7" customWidth="1"/>
-    <col min="16" max="17" width="52.5703125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="52.5703125" style="6" customWidth="1"/>
-    <col min="19" max="19" width="52.5703125" style="7" customWidth="1"/>
-    <col min="20" max="20" width="52.5703125" style="9" customWidth="1"/>
-    <col min="21" max="21" width="52.5703125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="52.5703125" style="9" customWidth="1"/>
-    <col min="23" max="24" width="52.5703125" style="6" customWidth="1"/>
-    <col min="25" max="25" width="52.5703125" style="9" customWidth="1"/>
-    <col min="26" max="26" width="52.5703125" style="6" customWidth="1"/>
-    <col min="27" max="27" width="52.5703125" style="7" customWidth="1"/>
-    <col min="28" max="28" width="52.5703125" style="6" customWidth="1"/>
-    <col min="29" max="1025" width="52.5703125" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" style="5"/>
+    <col min="8" max="8" width="52.5703125" style="4"/>
+    <col min="9" max="13" width="52.5703125" style="3"/>
+    <col min="14" max="14" width="52.5703125" style="6"/>
+    <col min="15" max="15" width="52.5703125" style="7"/>
+    <col min="16" max="17" width="52.5703125" style="8"/>
+    <col min="18" max="18" width="52.5703125" style="6"/>
+    <col min="19" max="19" width="52.5703125" style="7"/>
+    <col min="20" max="20" width="52.5703125" style="9"/>
+    <col min="21" max="21" width="52.5703125" style="7"/>
+    <col min="22" max="22" width="52.5703125" style="9"/>
+    <col min="23" max="24" width="52.5703125" style="6"/>
+    <col min="25" max="25" width="52.5703125" style="9"/>
+    <col min="26" max="26" width="52.5703125" style="6"/>
+    <col min="27" max="27" width="52.5703125" style="7"/>
+    <col min="28" max="28" width="52.5703125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="95.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1257,64 +1274,82 @@
         <v>9</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="O3" s="6"/>
       <c r="S3" s="6"/>
       <c r="U3" s="6"/>
@@ -4307,109 +4342,109 @@
       <formula1>8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite letras ou números._x000a_Até 15 caracteres." promptTitle="Informe a Inscrição Municipal" prompt="Digite letras ou números._x000a_Até 15 caracteres." sqref="I3:I1002" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite letras ou números._x000a_Até 15 caracteres." promptTitle="Informe a Inscrição Municipal" prompt="Digite letras ou números._x000a_Até 15 caracteres." sqref="I3:I1002" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>15</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite entre 2 a 14 números." promptTitle="Informe a Inscrição Estadual" prompt="Se Contribuinte, esse campo é obrigatório._x000a_Se Não contribuinte, esse campo é opcional._x000a_Se Isento, esse campo não deve ser preenchido._x000a_Digite entre 2 a 14 números." sqref="K3 K4:L1002" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite entre 2 a 14 números." promptTitle="Informe a Inscrição Estadual" prompt="Se Contribuinte, esse campo é obrigatório._x000a_Se Não contribuinte, esse campo é opcional._x000a_Se Isento, esse campo não deve ser preenchido._x000a_Digite entre 2 a 14 números." sqref="K3 K4:L1002" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>2</formula1>
       <formula2>14</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Selecione uma opção." promptTitle="Selecione o tipo do cadastro" prompt="Campo obrigatório._x000a_Selecione uma opção." sqref="J3:J1002" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Selecione uma opção." promptTitle="Selecione o tipo do cadastro" prompt="Campo obrigatório._x000a_Selecione uma opção." sqref="J3:J1002" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Contribuinte,Não contribuinte,Isento"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite entre 2 a 14 números." promptTitle="Informe o SUFRAMA" prompt="Só preencha se a UF da sua empresa for igual a Rondônia, Roraima, Acre ou Amapá._x000a_Digite letras ou números._x000a_Entre 2 a 14 caracteres." sqref="L3" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite entre 2 a 14 números." promptTitle="Informe o SUFRAMA" prompt="Só preencha se a UF da sua empresa for igual a Rondônia, Roraima, Acre ou Amapá._x000a_Digite letras ou números._x000a_Entre 2 a 14 caracteres." sqref="L3" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>8</formula1>
       <formula2>9</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite apenas 7 números." promptTitle="Digite o CNAE principal" prompt="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite apenas 7 números." sqref="H3:H1002" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite apenas 7 números." promptTitle="Digite o CNAE principal" prompt="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite apenas 7 números." sqref="H3:H1002" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite letras ou números._x000a_Entre 2 e 55 caracteres." promptTitle="Digite o Nome Fantasia" prompt="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite letras ou números._x000a_Entre 2 e 55 caracteres." sqref="F3:F1002" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite letras ou números._x000a_Entre 2 e 55 caracteres." promptTitle="Digite o Nome Fantasia" prompt="Só preencha se o perfil do parceiro for Pessoa Jurídica._x000a_Digite letras ou números._x000a_Entre 2 e 55 caracteres." sqref="F3:F1002" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>2</formula1>
       <formula2>55</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Só preencha se o perfil do parceiro for Pessoa Física._x000a_Digite apenas data." promptTitle="Digite a data de aniversário" prompt="Campo obrigatório._x000a_Só preencha se o perfil do parceiro for Pessoa Física._x000a_Digite apenas data." sqref="G3:G1002" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Só preencha se o perfil do parceiro for Pessoa Física._x000a_Digite apenas data." promptTitle="Digite a data de aniversário" prompt="Campo obrigatório._x000a_Só preencha se o perfil do parceiro for Pessoa Física._x000a_Digite apenas data." sqref="G3:G1002" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Pessoa Física - CPF de 11 números_x000a_Pessoa Jurídica - CNPJ de 14 números_x000a_Estrangeiro - Até 20 dígitos (letras ou números)" promptTitle="Digite o documento de identificação" prompt="Campo obrigatório._x000a_Se parceiro for Pessoa Física, insira CPF de 11 dígitos numéricos;_x000a_Se parceiro for Pessoa Jurídica insira CNPJ de 14 dígitos numéricos;_x000a_Se parceiro for Estrangeiro, insira um identificador de até 20 dígitos (letras ou números)." sqref="D3:D1002" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Pessoa Física - CPF de 11 números_x000a_Pessoa Jurídica - CNPJ de 14 números_x000a_Estrangeiro - Até 20 dígitos (letras ou números)" promptTitle="Digite o documento de identificação" prompt="Campo obrigatório._x000a_Se parceiro for Pessoa Física, insira CPF de 11 dígitos numéricos;_x000a_Se parceiro for Pessoa Jurídica insira CNPJ de 14 dígitos numéricos;_x000a_Se parceiro for Estrangeiro, insira um identificador de até 20 dígitos (letras ou números)." sqref="D3:D1002" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>20</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Selecione uma opção." promptTitle="Selecione o perfil do parceiro" prompt="Campo obrigatório._x000a_Selecione uma opção." sqref="C3:C1002" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Selecione uma opção." promptTitle="Selecione o perfil do parceiro" prompt="Campo obrigatório._x000a_Selecione uma opção." sqref="C3:C1002" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Pessoa Física,Pessoa Jurídica,Estrangeiro"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o nome do contato" prompt="Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="M3:M1002" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o nome do contato" prompt="Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="M3:M1002" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>60</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Se parceiro for Pessoa Física, insira CPF de 11 dígitos numéricos;_x000a_Se parceiro for Pessoa Jurídica insira CNPJ de 14 dígitos numéricos." promptTitle="Digite o documento do contato" prompt="Campo obrigatório._x000a_Se parceiro for Pessoa Física, insira CPF de 11 dígitos numéricos;_x000a_Se parceiro for Pessoa Jurídica insira CNPJ de 14 dígitos numéricos." sqref="N3:N1002" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Se parceiro for Pessoa Física, insira CPF de 11 dígitos numéricos;_x000a_Se parceiro for Pessoa Jurídica insira CNPJ de 14 dígitos numéricos." promptTitle="Digite o documento do contato" prompt="Campo obrigatório._x000a_Se parceiro for Pessoa Física, insira CPF de 11 dígitos numéricos;_x000a_Se parceiro for Pessoa Jurídica insira CNPJ de 14 dígitos numéricos." sqref="N3:N1002" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>11</formula1>
       <formula2>14</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção válida." promptTitle="Informe o tipo de telefone de contato" prompt="Selecione uma opção válida." sqref="Q3:Q1002" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção válida." promptTitle="Informe o tipo de telefone de contato" prompt="Selecione uma opção válida." sqref="Q3:Q1002" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>"Celular,Comercial,Residencial,FAX,Outros"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Somente números._x000a_Tamanho mínimo 10 e máximo 11." promptTitle="Informe o telefone do contato" prompt="Somente números._x000a_Tamanho mínimo 10 e máximo 11." sqref="R3:R1002" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Somente números._x000a_Tamanho mínimo 10 e máximo 11." promptTitle="Informe o telefone do contato" prompt="Somente números._x000a_Tamanho mínimo 10 e máximo 11." sqref="R3:R1002" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>10</formula1>
       <formula2>11</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o logradouro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o logradouro" prompt="Informe o logradouro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="V3:V1002" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o logradouro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o logradouro" prompt="Informe o logradouro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="V3:V1002" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>1</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção." promptTitle="Selecione o tipo do endereço" prompt="Selecione uma opção somente se você preencher o CEP do parceiro." sqref="T3:T1002" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção." promptTitle="Selecione o tipo do endereço" prompt="Selecione uma opção somente se você preencher o CEP do parceiro." sqref="T3:T1002" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"Comercial,Residencial,Cobrança,Entrega,Outros"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o número somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 10 caracteres." promptTitle="Informe o número" prompt="Informe o número somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 10 caracteres." sqref="W3:W1002" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o número somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 10 caracteres." promptTitle="Informe o número" prompt="Informe o número somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 10 caracteres." sqref="W3:W1002" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o complemento somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." promptTitle="Informe o complemento" prompt="Informe o complemento somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." sqref="X3:X1002" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o complemento somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." promptTitle="Informe o complemento" prompt="Informe o complemento somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." sqref="X3:X1002" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>1</formula1>
       <formula2>50</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o munícipio somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o município" prompt="Informe o munícipio somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="Y3:Y1002" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o munícipio somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o município" prompt="Informe o munícipio somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="Y3:Y1002" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>1</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o bairro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o bairro" prompt="Informe o bairro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="Z3:Z1002" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o bairro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." promptTitle="Informe o bairro" prompt="Informe o bairro somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 60 caracteres." sqref="Z3:Z1002" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>1</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o país somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." promptTitle="Informe o País" prompt="Informe o país somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." sqref="AB3:AB1002" xr:uid="{00000000-0002-0000-0000-000017000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Informe o país somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." promptTitle="Informe o País" prompt="Informe o país somente se você preencheu o CEP do parceiro._x000a_Digite letras ou números._x000a_Entre 1 e 50 caracteres." sqref="AB3:AB1002" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>1</formula1>
       <formula2>50</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Selecione uma opção." promptTitle="Selecione o tipo do cadastro" prompt="Campo obrigatório._x000a_Selecione uma opção." sqref="B3:B1002" xr:uid="{00000000-0002-0000-0000-000018000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Selecione uma opção." promptTitle="Selecione o tipo do cadastro" prompt="Campo obrigatório._x000a_Selecione uma opção." sqref="B3:B1002" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>"Cliente,Fornecedor,Transportadora,Cliente | Fornecedor,Cliente | Fornecedor | Transportadora,Cliente | Transportadora,Fornecedor | Transportadora"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Digite letras ou números._x000a_Entre 2 e 60 caracteres." promptTitle="Informe a razão social ou nome do parceiro" prompt="Campo obrigatório._x000a_Digite letras ou números._x000a_Entre 2 e 60 caracteres." sqref="E3:E1002" xr:uid="{00000000-0002-0000-0000-000019000000}">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Campo obrigatório._x000a_Digite letras ou números._x000a_Entre 2 e 60 caracteres." promptTitle="Informe a razão social ou nome do parceiro" prompt="Campo obrigatório._x000a_Digite letras ou números._x000a_Entre 2 e 60 caracteres." sqref="E3:E1002" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>2</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção válida." promptTitle="Este contato recebe XML?" prompt="Selecione uma opção válida." sqref="P3:P1002" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção válida." promptTitle="Este contato recebe XML?" prompt="Selecione uma opção válida." sqref="P3:P1002" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>"Sim,Não"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção válida." promptTitle="Informe o status do produto" prompt="Selecione uma opção válida." sqref="A3:A1002" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma opção válida." promptTitle="Informe o status do produto" prompt="Selecione uma opção válida." sqref="A3:A1002" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>"Ativo,Inativo"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma UF somente se você preencheu o CEP do fornecedor._x000a_" promptTitle="Selecione uma UF" prompt="Selecione uma UF somente se você preencheu o CEP do fornecedor._x000a_" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ops! Algo deu errado" error="Selecione uma UF somente se você preencheu o CEP do fornecedor._x000a_" promptTitle="Selecione uma UF" prompt="Selecione uma UF somente se você preencheu o CEP do fornecedor._x000a_" xr:uid="{00000000-0002-0000-0000-00001B000000}">
           <x14:formula1>
             <xm:f>Planilha1!$A$2:$A$28</xm:f>
           </x14:formula1>
@@ -4432,155 +4467,154 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="14" customWidth="1"/>
-    <col min="2" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -4592,394 +4626,391 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="94" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>